<commit_message>
fixed question 3, working on 8
</commit_message>
<xml_diff>
--- a/metro_budget_exercise.xlsx
+++ b/metro_budget_exercise.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\melan\Documents\DA8\Projects\budget_lookups-melaniewesson\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9B5A013-1094-4772-BD12-661FDABFE6A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B560A507-0E93-4927-9812-BF189CCF07B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2463,7 +2463,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A68" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
       <selection activeCell="B92" sqref="B92"/>
     </sheetView>
   </sheetViews>
@@ -2550,7 +2550,7 @@
         <v>-4.3170750765267295E-2</v>
       </c>
       <c r="F2">
-        <f>RANK(E2,E2:E52,1)</f>
+        <f>RANK(E2,$E$2:$E$52,1)</f>
         <v>14</v>
       </c>
       <c r="G2">
@@ -2568,7 +2568,7 @@
         <v>-9.4972027086493035E-2</v>
       </c>
       <c r="K2">
-        <f>RANK(J2,J2:J52,1)</f>
+        <f>RANK(J2,$J$2:$J$52,1)</f>
         <v>10</v>
       </c>
       <c r="L2">
@@ -2586,7 +2586,7 @@
         <v>-5.6484362894991494E-2</v>
       </c>
       <c r="P2">
-        <f>RANK(O2,O2:O52,1)</f>
+        <f>RANK(O2,$O$2:$O$52,1)</f>
         <v>14</v>
       </c>
     </row>
@@ -2609,8 +2609,8 @@
         <v>-2.3069981751824741E-2</v>
       </c>
       <c r="F3">
-        <f t="shared" ref="F3:F52" si="2">RANK(E3,E3:E53,1)</f>
-        <v>21</v>
+        <f t="shared" ref="F3:F52" si="2">RANK(E3,$E$2:$E$52,1)</f>
+        <v>22</v>
       </c>
       <c r="G3">
         <v>334800</v>
@@ -2627,8 +2627,8 @@
         <v>-6.6804928315415249E-2</v>
       </c>
       <c r="K3">
-        <f t="shared" ref="K3:K52" si="5">RANK(J3,J3:J53,1)</f>
-        <v>13</v>
+        <f t="shared" ref="K3:K52" si="5">RANK(J3,$J$2:$J$52,1)</f>
+        <v>14</v>
       </c>
       <c r="L3">
         <v>322700</v>
@@ -2645,8 +2645,8 @@
         <v>-1.3540749922529313E-3</v>
       </c>
       <c r="P3">
-        <f t="shared" ref="P3:P52" si="8">RANK(O3,O3:O53,1)</f>
-        <v>36</v>
+        <f t="shared" ref="P3:P52" si="8">RANK(O3,$O$2:$O$52,1)</f>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
@@ -2669,7 +2669,7 @@
       </c>
       <c r="F4">
         <f t="shared" si="2"/>
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="G4">
         <v>3652300</v>
@@ -2687,7 +2687,7 @@
       </c>
       <c r="K4">
         <f t="shared" si="5"/>
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="L4">
         <v>3662400</v>
@@ -2705,7 +2705,7 @@
       </c>
       <c r="P4">
         <f t="shared" si="8"/>
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
@@ -2764,7 +2764,7 @@
       </c>
       <c r="P5">
         <f t="shared" si="8"/>
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
@@ -2787,7 +2787,7 @@
       </c>
       <c r="F6">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G6">
         <v>428500</v>
@@ -2805,7 +2805,7 @@
       </c>
       <c r="K6">
         <f t="shared" si="5"/>
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="L6">
         <v>445200</v>
@@ -2823,7 +2823,7 @@
       </c>
       <c r="P6">
         <f t="shared" si="8"/>
-        <v>35</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
@@ -2864,7 +2864,7 @@
       </c>
       <c r="K7">
         <f t="shared" si="5"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="L7">
         <v>3345200</v>
@@ -2964,7 +2964,7 @@
       </c>
       <c r="F9">
         <f t="shared" si="2"/>
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="G9">
         <v>11073700</v>
@@ -2982,7 +2982,7 @@
       </c>
       <c r="K9">
         <f t="shared" si="5"/>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="L9">
         <v>10790500</v>
@@ -3000,7 +3000,7 @@
       </c>
       <c r="P9">
         <f t="shared" si="8"/>
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
@@ -3023,7 +3023,7 @@
       </c>
       <c r="F10">
         <f t="shared" si="2"/>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G10">
         <v>495200</v>
@@ -3041,7 +3041,7 @@
       </c>
       <c r="K10">
         <f t="shared" si="5"/>
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="L10">
         <v>487500</v>
@@ -3059,7 +3059,7 @@
       </c>
       <c r="P10">
         <f t="shared" si="8"/>
-        <v>23</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
@@ -3082,7 +3082,7 @@
       </c>
       <c r="F11">
         <f t="shared" si="2"/>
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="G11">
         <v>0</v>
@@ -3100,7 +3100,7 @@
       </c>
       <c r="K11">
         <f t="shared" si="5"/>
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="L11">
         <v>375000</v>
@@ -3141,7 +3141,7 @@
       </c>
       <c r="F12">
         <f t="shared" si="2"/>
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="G12">
         <v>4700400</v>
@@ -3159,7 +3159,7 @@
       </c>
       <c r="K12">
         <f t="shared" si="5"/>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="L12">
         <v>4677800</v>
@@ -3177,7 +3177,7 @@
       </c>
       <c r="P12">
         <f t="shared" si="8"/>
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
@@ -3200,7 +3200,7 @@
       </c>
       <c r="F13">
         <f t="shared" si="2"/>
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="G13">
         <v>6223700</v>
@@ -3218,7 +3218,7 @@
       </c>
       <c r="K13">
         <f t="shared" si="5"/>
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="L13">
         <v>6207300</v>
@@ -3236,7 +3236,7 @@
       </c>
       <c r="P13">
         <f t="shared" si="8"/>
-        <v>19</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
@@ -3259,7 +3259,7 @@
       </c>
       <c r="F14">
         <f t="shared" si="2"/>
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="G14">
         <v>530500</v>
@@ -3277,7 +3277,7 @@
       </c>
       <c r="K14">
         <f t="shared" si="5"/>
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="L14">
         <v>526200</v>
@@ -3295,7 +3295,7 @@
       </c>
       <c r="P14">
         <f t="shared" si="8"/>
-        <v>13</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
@@ -3318,7 +3318,7 @@
       </c>
       <c r="F15">
         <f t="shared" si="2"/>
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="G15">
         <v>184167800</v>
@@ -3336,7 +3336,7 @@
       </c>
       <c r="K15">
         <f t="shared" si="5"/>
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="L15">
         <v>188953500</v>
@@ -3354,7 +3354,7 @@
       </c>
       <c r="P15">
         <f t="shared" si="8"/>
-        <v>18</v>
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
@@ -3377,7 +3377,7 @@
       </c>
       <c r="F16">
         <f t="shared" si="2"/>
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="G16">
         <v>7352500</v>
@@ -3395,7 +3395,7 @@
       </c>
       <c r="K16">
         <f t="shared" si="5"/>
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="L16">
         <v>7397200</v>
@@ -3413,7 +3413,7 @@
       </c>
       <c r="P16">
         <f t="shared" si="8"/>
-        <v>29</v>
+        <v>43</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
@@ -3436,7 +3436,7 @@
       </c>
       <c r="F17">
         <f t="shared" si="2"/>
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="G17">
         <v>15309700</v>
@@ -3454,7 +3454,7 @@
       </c>
       <c r="K17">
         <f t="shared" si="5"/>
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="L17">
         <v>15311800</v>
@@ -3472,7 +3472,7 @@
       </c>
       <c r="P17">
         <f t="shared" si="8"/>
-        <v>6</v>
+        <v>11</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
@@ -3495,7 +3495,7 @@
       </c>
       <c r="F18">
         <f t="shared" si="2"/>
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="G18">
         <v>2861000</v>
@@ -3513,7 +3513,7 @@
       </c>
       <c r="K18">
         <f t="shared" si="5"/>
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="L18">
         <v>2910600</v>
@@ -3531,7 +3531,7 @@
       </c>
       <c r="P18">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
@@ -3554,7 +3554,7 @@
       </c>
       <c r="F19">
         <f t="shared" si="2"/>
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="G19">
         <v>9713300</v>
@@ -3572,7 +3572,7 @@
       </c>
       <c r="K19">
         <f t="shared" si="5"/>
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="L19">
         <v>9343000</v>
@@ -3590,7 +3590,7 @@
       </c>
       <c r="P19">
         <f t="shared" si="8"/>
-        <v>5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
@@ -3613,7 +3613,7 @@
       </c>
       <c r="F20">
         <f t="shared" si="2"/>
-        <v>30</v>
+        <v>46</v>
       </c>
       <c r="G20">
         <v>131849400</v>
@@ -3631,7 +3631,7 @@
       </c>
       <c r="K20">
         <f t="shared" si="5"/>
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="L20">
         <v>130621400</v>
@@ -3649,7 +3649,7 @@
       </c>
       <c r="P20">
         <f t="shared" si="8"/>
-        <v>28</v>
+        <v>46</v>
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">
@@ -3672,7 +3672,7 @@
       </c>
       <c r="F21">
         <f t="shared" si="2"/>
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="G21">
         <v>24497400</v>
@@ -3690,7 +3690,7 @@
       </c>
       <c r="K21">
         <f t="shared" si="5"/>
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="L21">
         <v>24323000</v>
@@ -3708,7 +3708,7 @@
       </c>
       <c r="P21">
         <f t="shared" si="8"/>
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
@@ -3731,7 +3731,7 @@
       </c>
       <c r="F22">
         <f t="shared" si="2"/>
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="G22">
         <v>11980700</v>
@@ -3749,7 +3749,7 @@
       </c>
       <c r="K22">
         <f t="shared" si="5"/>
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="L22">
         <v>11935200</v>
@@ -3767,7 +3767,7 @@
       </c>
       <c r="P22">
         <f t="shared" si="8"/>
-        <v>24</v>
+        <v>42</v>
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
@@ -3790,7 +3790,7 @@
       </c>
       <c r="F23">
         <f t="shared" si="2"/>
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="G23">
         <v>22683800</v>
@@ -3808,7 +3808,7 @@
       </c>
       <c r="K23">
         <f t="shared" si="5"/>
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="L23">
         <v>23220300</v>
@@ -3826,7 +3826,7 @@
       </c>
       <c r="P23">
         <f t="shared" si="8"/>
-        <v>13</v>
+        <v>26</v>
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
@@ -3849,7 +3849,7 @@
       </c>
       <c r="F24">
         <f t="shared" si="2"/>
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="G24">
         <v>1112700</v>
@@ -3867,7 +3867,7 @@
       </c>
       <c r="K24">
         <f t="shared" si="5"/>
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="L24">
         <v>1112600</v>
@@ -3885,7 +3885,7 @@
       </c>
       <c r="P24">
         <f t="shared" si="8"/>
-        <v>22</v>
+        <v>41</v>
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
@@ -3908,7 +3908,7 @@
       </c>
       <c r="F25">
         <f t="shared" si="2"/>
-        <v>19</v>
+        <v>38</v>
       </c>
       <c r="G25">
         <v>505200</v>
@@ -3926,7 +3926,7 @@
       </c>
       <c r="K25">
         <f t="shared" si="5"/>
-        <v>20</v>
+        <v>37</v>
       </c>
       <c r="L25">
         <v>496500</v>
@@ -3944,7 +3944,7 @@
       </c>
       <c r="P25">
         <f t="shared" si="8"/>
-        <v>18</v>
+        <v>35</v>
       </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.25">
@@ -3967,7 +3967,7 @@
       </c>
       <c r="F26">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G26">
         <v>5442200</v>
@@ -3985,7 +3985,7 @@
       </c>
       <c r="K26">
         <f t="shared" si="5"/>
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="L26">
         <v>5430700</v>
@@ -4003,7 +4003,7 @@
       </c>
       <c r="P26">
         <f t="shared" si="8"/>
-        <v>5</v>
+        <v>13</v>
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.25">
@@ -4026,7 +4026,7 @@
       </c>
       <c r="F27">
         <f t="shared" si="2"/>
-        <v>24</v>
+        <v>47</v>
       </c>
       <c r="G27">
         <v>0</v>
@@ -4044,7 +4044,7 @@
       </c>
       <c r="K27">
         <f t="shared" si="5"/>
-        <v>24</v>
+        <v>48</v>
       </c>
       <c r="L27">
         <v>0</v>
@@ -4062,7 +4062,7 @@
       </c>
       <c r="P27">
         <f t="shared" si="8"/>
-        <v>23</v>
+        <v>48</v>
       </c>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.25">
@@ -4085,7 +4085,7 @@
       </c>
       <c r="F28">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G28">
         <v>1545700</v>
@@ -4121,7 +4121,7 @@
       </c>
       <c r="P28">
         <f t="shared" si="8"/>
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.25">
@@ -4144,7 +4144,7 @@
       </c>
       <c r="F29">
         <f t="shared" si="2"/>
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="G29">
         <v>2779500</v>
@@ -4162,7 +4162,7 @@
       </c>
       <c r="K29">
         <f t="shared" si="5"/>
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="L29">
         <v>2889900</v>
@@ -4180,7 +4180,7 @@
       </c>
       <c r="P29">
         <f t="shared" si="8"/>
-        <v>19</v>
+        <v>44</v>
       </c>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.25">
@@ -4203,7 +4203,7 @@
       </c>
       <c r="F30">
         <f t="shared" si="2"/>
-        <v>17</v>
+        <v>40</v>
       </c>
       <c r="G30">
         <v>12735900</v>
@@ -4221,7 +4221,7 @@
       </c>
       <c r="K30">
         <f t="shared" si="5"/>
-        <v>19</v>
+        <v>42</v>
       </c>
       <c r="L30">
         <v>12861300</v>
@@ -4239,7 +4239,7 @@
       </c>
       <c r="P30">
         <f t="shared" si="8"/>
-        <v>16</v>
+        <v>36</v>
       </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.25">
@@ -4262,7 +4262,7 @@
       </c>
       <c r="F31">
         <f t="shared" si="2"/>
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="G31">
         <v>1823300</v>
@@ -4280,7 +4280,7 @@
       </c>
       <c r="K31">
         <f t="shared" si="5"/>
-        <v>13</v>
+        <v>32</v>
       </c>
       <c r="L31">
         <v>1870700</v>
@@ -4298,7 +4298,7 @@
       </c>
       <c r="P31">
         <f t="shared" si="8"/>
-        <v>8</v>
+        <v>20</v>
       </c>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.25">
@@ -4321,7 +4321,7 @@
       </c>
       <c r="F32">
         <f t="shared" si="2"/>
-        <v>14</v>
+        <v>36</v>
       </c>
       <c r="G32">
         <v>6195500</v>
@@ -4339,7 +4339,7 @@
       </c>
       <c r="K32">
         <f t="shared" si="5"/>
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="L32">
         <v>6157400</v>
@@ -4357,7 +4357,7 @@
       </c>
       <c r="P32">
         <f t="shared" si="8"/>
-        <v>8</v>
+        <v>23</v>
       </c>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.25">
@@ -4380,7 +4380,7 @@
       </c>
       <c r="F33">
         <f t="shared" si="2"/>
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="G33">
         <v>979671000</v>
@@ -4398,7 +4398,7 @@
       </c>
       <c r="K33">
         <f t="shared" si="5"/>
-        <v>17</v>
+        <v>43</v>
       </c>
       <c r="L33">
         <v>989572899.99999905</v>
@@ -4416,7 +4416,7 @@
       </c>
       <c r="P33">
         <f t="shared" si="8"/>
-        <v>13</v>
+        <v>34</v>
       </c>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.25">
@@ -4439,7 +4439,7 @@
       </c>
       <c r="F34">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="G34">
         <v>4350600</v>
@@ -4457,7 +4457,7 @@
       </c>
       <c r="K34">
         <f t="shared" si="5"/>
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="L34">
         <v>4345600</v>
@@ -4475,7 +4475,7 @@
       </c>
       <c r="P34">
         <f t="shared" si="8"/>
-        <v>8</v>
+        <v>24</v>
       </c>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.25">
@@ -4498,7 +4498,7 @@
       </c>
       <c r="F35">
         <f t="shared" si="2"/>
-        <v>17</v>
+        <v>47</v>
       </c>
       <c r="G35">
         <v>0</v>
@@ -4516,7 +4516,7 @@
       </c>
       <c r="K35">
         <f t="shared" si="5"/>
-        <v>17</v>
+        <v>48</v>
       </c>
       <c r="L35">
         <v>0</v>
@@ -4534,7 +4534,7 @@
       </c>
       <c r="P35">
         <f t="shared" si="8"/>
-        <v>16</v>
+        <v>48</v>
       </c>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.25">
@@ -4557,7 +4557,7 @@
       </c>
       <c r="F36">
         <f t="shared" si="2"/>
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="G36">
         <v>898700</v>
@@ -4593,7 +4593,7 @@
       </c>
       <c r="P36">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.25">
@@ -4616,7 +4616,7 @@
       </c>
       <c r="F37">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="G37">
         <v>2229200</v>
@@ -4634,7 +4634,7 @@
       </c>
       <c r="K37">
         <f t="shared" si="5"/>
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="L37">
         <v>2296900</v>
@@ -4652,7 +4652,7 @@
       </c>
       <c r="P37">
         <f t="shared" si="8"/>
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.25">
@@ -4675,7 +4675,7 @@
       </c>
       <c r="F38">
         <f t="shared" si="2"/>
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="G38">
         <v>792800</v>
@@ -4693,7 +4693,7 @@
       </c>
       <c r="K38">
         <f t="shared" si="5"/>
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="L38">
         <v>777800</v>
@@ -4711,7 +4711,7 @@
       </c>
       <c r="P38">
         <f t="shared" si="8"/>
-        <v>11</v>
+        <v>40</v>
       </c>
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.25">
@@ -4734,7 +4734,7 @@
       </c>
       <c r="F39">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="G39">
         <v>1294400</v>
@@ -4752,7 +4752,7 @@
       </c>
       <c r="K39">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L39">
         <v>1759500</v>
@@ -4770,7 +4770,7 @@
       </c>
       <c r="P39">
         <f t="shared" si="8"/>
-        <v>4</v>
+        <v>17</v>
       </c>
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.25">
@@ -4793,7 +4793,7 @@
       </c>
       <c r="F40">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="G40">
         <v>39964900</v>
@@ -4811,7 +4811,7 @@
       </c>
       <c r="K40">
         <f t="shared" si="5"/>
-        <v>3</v>
+        <v>22</v>
       </c>
       <c r="L40">
         <v>40216700</v>
@@ -4829,7 +4829,7 @@
       </c>
       <c r="P40">
         <f t="shared" si="8"/>
-        <v>6</v>
+        <v>31</v>
       </c>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.25">
@@ -4852,7 +4852,7 @@
       </c>
       <c r="F41">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="G41">
         <v>5089500</v>
@@ -4870,7 +4870,7 @@
       </c>
       <c r="K41">
         <f t="shared" si="5"/>
-        <v>8</v>
+        <v>34</v>
       </c>
       <c r="L41">
         <v>4799900</v>
@@ -4888,7 +4888,7 @@
       </c>
       <c r="P41">
         <f t="shared" si="8"/>
-        <v>5</v>
+        <v>30</v>
       </c>
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.25">
@@ -4911,7 +4911,7 @@
       </c>
       <c r="F42">
         <f t="shared" si="2"/>
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="G42">
         <v>199130300</v>
@@ -4929,7 +4929,7 @@
       </c>
       <c r="K42">
         <f t="shared" si="5"/>
-        <v>8</v>
+        <v>39</v>
       </c>
       <c r="L42">
         <v>199954600</v>
@@ -4947,7 +4947,7 @@
       </c>
       <c r="P42">
         <f t="shared" si="8"/>
-        <v>9</v>
+        <v>47</v>
       </c>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.25">
@@ -4970,7 +4970,7 @@
       </c>
       <c r="F43">
         <f t="shared" si="2"/>
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="G43">
         <v>8560800</v>
@@ -4988,7 +4988,7 @@
       </c>
       <c r="K43">
         <f t="shared" si="5"/>
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="L43">
         <v>8497500</v>
@@ -5006,7 +5006,7 @@
       </c>
       <c r="P43">
         <f t="shared" si="8"/>
-        <v>4</v>
+        <v>18</v>
       </c>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.25">
@@ -5029,7 +5029,7 @@
       </c>
       <c r="F44">
         <f t="shared" si="2"/>
-        <v>6</v>
+        <v>39</v>
       </c>
       <c r="G44">
         <v>31040700</v>
@@ -5047,7 +5047,7 @@
       </c>
       <c r="K44">
         <f t="shared" si="5"/>
-        <v>7</v>
+        <v>41</v>
       </c>
       <c r="L44">
         <v>31282200</v>
@@ -5065,7 +5065,7 @@
       </c>
       <c r="P44">
         <f t="shared" si="8"/>
-        <v>7</v>
+        <v>45</v>
       </c>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.25">
@@ -5088,7 +5088,7 @@
       </c>
       <c r="F45">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>34</v>
       </c>
       <c r="G45">
         <v>56792200</v>
@@ -5106,7 +5106,7 @@
       </c>
       <c r="K45">
         <f t="shared" si="5"/>
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="L45">
         <v>56027100</v>
@@ -5124,7 +5124,7 @@
       </c>
       <c r="P45">
         <f t="shared" si="8"/>
-        <v>4</v>
+        <v>32</v>
       </c>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.25">
@@ -5147,7 +5147,7 @@
       </c>
       <c r="F46">
         <f t="shared" si="2"/>
-        <v>5</v>
+        <v>43</v>
       </c>
       <c r="G46">
         <v>266000</v>
@@ -5165,7 +5165,7 @@
       </c>
       <c r="K46">
         <f t="shared" si="5"/>
-        <v>5</v>
+        <v>33</v>
       </c>
       <c r="L46">
         <v>267100</v>
@@ -5183,7 +5183,7 @@
       </c>
       <c r="P46">
         <f t="shared" si="8"/>
-        <v>3</v>
+        <v>16</v>
       </c>
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.25">
@@ -5206,7 +5206,7 @@
       </c>
       <c r="F47">
         <f t="shared" si="2"/>
-        <v>5</v>
+        <v>45</v>
       </c>
       <c r="G47">
         <v>73467000</v>
@@ -5224,7 +5224,7 @@
       </c>
       <c r="K47">
         <f t="shared" si="5"/>
-        <v>5</v>
+        <v>45</v>
       </c>
       <c r="L47">
         <v>75072800</v>
@@ -5242,7 +5242,7 @@
       </c>
       <c r="P47">
         <f t="shared" si="8"/>
-        <v>4</v>
+        <v>38</v>
       </c>
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.25">
@@ -5265,7 +5265,7 @@
       </c>
       <c r="F48">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="G48">
         <v>7214700</v>
@@ -5283,7 +5283,7 @@
       </c>
       <c r="K48">
         <f t="shared" si="5"/>
-        <v>3</v>
+        <v>29</v>
       </c>
       <c r="L48">
         <v>7289800</v>
@@ -5301,7 +5301,7 @@
       </c>
       <c r="P48">
         <f t="shared" si="8"/>
-        <v>2</v>
+        <v>15</v>
       </c>
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.25">
@@ -5324,7 +5324,7 @@
       </c>
       <c r="F49">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>27</v>
       </c>
       <c r="G49">
         <v>102600</v>
@@ -5342,7 +5342,7 @@
       </c>
       <c r="K49">
         <f t="shared" si="5"/>
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="L49">
         <v>0</v>
@@ -5360,7 +5360,7 @@
       </c>
       <c r="P49">
         <f t="shared" si="8"/>
-        <v>3</v>
+        <v>48</v>
       </c>
     </row>
     <row r="50" spans="1:16" x14ac:dyDescent="0.25">
@@ -5383,7 +5383,7 @@
       </c>
       <c r="F50">
         <f t="shared" si="2"/>
-        <v>3</v>
+        <v>47</v>
       </c>
       <c r="G50">
         <v>859100</v>
@@ -5401,7 +5401,7 @@
       </c>
       <c r="K50">
         <f t="shared" si="5"/>
-        <v>3</v>
+        <v>48</v>
       </c>
       <c r="L50">
         <v>843200</v>
@@ -5419,7 +5419,7 @@
       </c>
       <c r="P50">
         <f t="shared" si="8"/>
-        <v>3</v>
+        <v>48</v>
       </c>
     </row>
     <row r="51" spans="1:16" x14ac:dyDescent="0.25">
@@ -5442,7 +5442,7 @@
       </c>
       <c r="F51">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>35</v>
       </c>
       <c r="G51">
         <v>8925500</v>
@@ -5460,7 +5460,7 @@
       </c>
       <c r="K51">
         <f t="shared" si="5"/>
-        <v>2</v>
+        <v>31</v>
       </c>
       <c r="L51">
         <v>8833900</v>
@@ -5478,7 +5478,7 @@
       </c>
       <c r="P51">
         <f t="shared" si="8"/>
-        <v>2</v>
+        <v>33</v>
       </c>
     </row>
     <row r="52" spans="1:16" x14ac:dyDescent="0.25">
@@ -5501,7 +5501,7 @@
       </c>
       <c r="F52">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="G52">
         <v>2440700</v>
@@ -5519,7 +5519,7 @@
       </c>
       <c r="K52">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="L52">
         <v>2321600</v>
@@ -5537,7 +5537,7 @@
       </c>
       <c r="P52">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="54" spans="1:16" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
finished question 8 part 1
</commit_message>
<xml_diff>
--- a/metro_budget_exercise.xlsx
+++ b/metro_budget_exercise.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\melan\Documents\DA8\Projects\budget_lookups-melaniewesson\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B560A507-0E93-4927-9812-BF189CCF07B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2144C714-28A6-4461-B89A-93B443BC8E78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,28 +32,6 @@
     </ext>
   </extLst>
 </workbook>
-</file>
-
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
-    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLDAPR" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
-          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <cellMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </cellMetadata>
-</metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2464,7 +2442,7 @@
   <dimension ref="A1:P100"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="B92" sqref="B92"/>
+      <selection activeCell="B101" sqref="B101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5907,17 +5885,17 @@
         <v>-82077.349999999627</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" s="7" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B83" s="1" t="s">
         <v>71</v>
       </c>
@@ -5925,7 +5903,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>73</v>
       </c>
@@ -5938,7 +5916,7 @@
         <v>385908.52</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>74</v>
       </c>
@@ -5951,7 +5929,7 @@
         <v>427758.64</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>75</v>
       </c>
@@ -5964,7 +5942,7 @@
         <v>445114.28999999899</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>0</v>
       </c>
@@ -5972,12 +5950,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" s="7" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>77</v>
       </c>
@@ -5993,7 +5971,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B90" s="8" t="s">
         <v>0</v>
       </c>
@@ -6013,52 +5991,99 @@
         <v>78</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>5</v>
       </c>
-      <c r="B91" t="e" cm="1">
-        <f t="array" ref="B91">_xlfn.XLOOKUP(B$89, (INDEX($B$2:$P$52, (MATCH($A91, $A$1:$P$1,0)))), A2:A52)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="C91" s="5"/>
-      <c r="E91" s="5"/>
-      <c r="G91" s="5"/>
-      <c r="H91" t="e">
-        <f>_xlfn.XLOOKUP(B$89,$A$2:$P$52,(MATCH($A91,$A$1:$P$1,0)))</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B91" t="str">
+        <f>_xlfn.XLOOKUP($B$89,F2:F52,A2:A52)</f>
+        <v>Clerk and Master - Chancery</v>
+      </c>
+      <c r="C91">
+        <f>_xlfn.XLOOKUP($B$89,F2:F52,E2:E52)</f>
+        <v>-0.15235918433091292</v>
+      </c>
+      <c r="D91" t="str">
+        <f>_xlfn.XLOOKUP($D$89,F2:F52,$A$2:$A$52)</f>
+        <v>Circuit Court Clerk</v>
+      </c>
+      <c r="E91">
+        <f>_xlfn.XLOOKUP($D$89,F2:F52, E2:E52)</f>
+        <v>-0.11502817362571344</v>
+      </c>
+      <c r="F91" t="str">
+        <f>_xlfn.XLOOKUP($F$89,F2:F52,A2:A52)</f>
+        <v>Internal Audit</v>
+      </c>
+      <c r="G91">
+        <f>_xlfn.XLOOKUP(F89,F2:F52,E2:E52)</f>
+        <v>-9.5782760864849215E-2</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>10</v>
       </c>
       <c r="B92" t="str">
-        <f t="shared" ref="B92:B93" si="14">_xlfn.XLOOKUP((RANK(B$89,F3:F53,1)),F3:F53,A3:A53)</f>
+        <f t="shared" ref="B92:C92" si="14">_xlfn.XLOOKUP($B$89,F3:F53,A3:A53)</f>
         <v>Clerk and Master - Chancery</v>
       </c>
-      <c r="C92" s="5"/>
-      <c r="E92" s="5"/>
-      <c r="G92" s="5"/>
-    </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C92">
+        <f>_xlfn.XLOOKUP($B$89, K2:K52,J2:J52)</f>
+        <v>-0.17551246244575608</v>
+      </c>
+      <c r="D92" t="str">
+        <f>_xlfn.XLOOKUP($D$89,K1:K52, $A$1:$A$52)</f>
+        <v>Internal Audit</v>
+      </c>
+      <c r="E92">
+        <f>_xlfn.XLOOKUP($D$89,K2:K52,J2:J52)</f>
+        <v>-0.17103239309050916</v>
+      </c>
+      <c r="F92" t="str">
+        <f>_xlfn.XLOOKUP($F$89, K2:K52,A2:A52)</f>
+        <v>Office of Family Safety</v>
+      </c>
+      <c r="G92">
+        <f>_xlfn.XLOOKUP(F89,K2:K52,J2:J52)</f>
+        <v>-0.13918241656366656</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>15</v>
       </c>
       <c r="B93" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" ref="B93:C93" si="15">_xlfn.XLOOKUP($B$89,F4:F54,A4:A54)</f>
         <v>Clerk and Master - Chancery</v>
       </c>
-      <c r="C93" s="5"/>
-      <c r="E93" s="5"/>
-      <c r="G93" s="5"/>
-    </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C93">
+        <f>_xlfn.XLOOKUP($B$89,P2:P52,O2:O52)</f>
+        <v>-0.82994157333333329</v>
+      </c>
+      <c r="D93" t="str">
+        <f>_xlfn.XLOOKUP($D$89,P2:P52, A2:A52)</f>
+        <v>Clerk and Master - Chancery</v>
+      </c>
+      <c r="E93">
+        <f>_xlfn.XLOOKUP($D$89,P2:P52,O2:O52)</f>
+        <v>-0.15295680364719175</v>
+      </c>
+      <c r="F93" t="str">
+        <f>_xlfn.XLOOKUP(F89,P2:P52,A2:A52)</f>
+        <v>Election Commission</v>
+      </c>
+      <c r="G93">
+        <f>_xlfn.XLOOKUP(F89,P2:P52,O2:O52)</f>
+        <v>-0.12882667147667154</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" s="7" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>77</v>
       </c>
@@ -6122,7 +6147,7 @@
       <c r="I100" s="4"/>
     </row>
   </sheetData>
-  <dataValidations count="2">
+  <dataValidations disablePrompts="1" count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A83" xr:uid="{0ECE0BAD-DC74-4E7B-8842-0609702F3664}">
       <formula1>$A$2:$A$52</formula1>
     </dataValidation>
@@ -6132,7 +6157,7 @@
   <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="1">
         <x14:dataValidation type="list" showInputMessage="1" prompt="Select department" xr:uid="{AEAF6F94-D033-427D-8D66-5F6FB454E309}">
           <x14:formula1>
             <xm:f>Departments!$A$2:$A$52</xm:f>

</xml_diff>